<commit_message>
Feat: LanguagePack UI Update
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Localization/English.xlsx
+++ b/Assets/StreamingAssets/Localization/English.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nbcamp\AirNHook\Assets\StreamingAssets\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55A4FB-6BC7-479D-9237-232E6F9C32C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3254FF-531E-40F2-A66E-43262E705194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10575" yWindow="2970" windowWidth="21600" windowHeight="11385" xr2:uid="{03AB7020-0D5B-4C42-B659-F913FE2E7807}"/>
+    <workbookView xWindow="-22410" yWindow="3645" windowWidth="21600" windowHeight="11385" xr2:uid="{03AB7020-0D5B-4C42-B659-F913FE2E7807}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>WindowMode</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Master</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -119,6 +115,38 @@
   </si>
   <si>
     <t>BGM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Failed to Connect</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RETRY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vsync</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resolution</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>APPLY CHANGE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>This option is not available in menu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullScreen</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -126,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +188,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -199,7 +234,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -213,6 +248,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,18 +587,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D177C49-BEC9-445E-96B9-01949D401546}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="17.25" thickBot="1">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -576,7 +614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17.25" thickBot="1">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
@@ -584,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="17.25" thickBot="1">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
@@ -592,7 +630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="17.25" thickBot="1">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
@@ -600,7 +638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="17.25" thickBot="1">
       <c r="A6" s="1">
         <v>1004</v>
       </c>
@@ -608,7 +646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="17.25" thickBot="1">
       <c r="A7" s="1">
         <v>1005</v>
       </c>
@@ -616,107 +654,163 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="17.25" thickBot="1">
       <c r="A8" s="1">
         <v>1006</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17.25" thickBot="1">
       <c r="A9" s="1">
         <v>1007</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17.25" thickBot="1">
       <c r="A10" s="1">
         <v>1008</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.25" thickBot="1">
       <c r="A11" s="1">
         <v>1009</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A12" s="1">
+        <v>1010</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A13" s="1">
+        <v>1011</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A14" s="1">
+        <v>1012</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A15" s="1">
+        <v>1013</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A16" s="1">
+        <v>1014</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A17" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A18" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A19" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A20" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A21" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2001</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2002</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>3001</v>
-      </c>
-      <c r="B16" s="3" t="s">
+    <row r="22" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A22" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A23" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>3002</v>
-      </c>
-      <c r="B17" s="3" t="s">
+    <row r="24" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A24" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>3003</v>
-      </c>
-      <c r="B18" s="2" t="s">
+    <row r="25" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A25" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="26" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A26" s="1">
         <v>4001</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="27" spans="1:2" ht="17.25" thickBot="1">
+      <c r="A27" s="1">
         <v>4002</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>